<commit_message>
Updated power requirement estimates
</commit_message>
<xml_diff>
--- a/power.xlsx
+++ b/power.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Landon\Documents\University of Akron\SDP\autocoffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA55182-86B1-41C7-80B3-E5D76A5D3253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7883AEFE-2F4D-44E0-8760-77058B03B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14670" yWindow="1980" windowWidth="26265" windowHeight="17730" xr2:uid="{7D14E45A-903B-472E-A95B-4E24BFDB7F5E}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D2:D6"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>